<commit_message>
Averages and standard deviations :)
</commit_message>
<xml_diff>
--- a/FTC Stats 2024/Red Team Data.xlsx
+++ b/FTC Stats 2024/Red Team Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Desktop\FTC 2024\FTC-Stats-2024\FTC Stats 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C80BEB4-659B-40C2-98F8-895866B15E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9714DE0-76B2-4EB0-B156-33DC03DC9092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{70A3623C-5B28-4542-A549-36E12E55390C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="28">
   <si>
     <t>Cas</t>
   </si>
@@ -492,21 +492,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4673F6C2-6DDF-48DA-81FA-878F968D73F6}">
-  <dimension ref="A1:Q77"/>
+  <dimension ref="A1:S77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="Q48" sqref="Q48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="11" max="11" width="12.42578125" customWidth="1"/>
     <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" customWidth="1"/>
     <col min="16" max="16" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
         <v>4</v>
@@ -544,11 +545,11 @@
       <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="N1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45587</v>
       </c>
@@ -582,12 +583,12 @@
       <c r="M3">
         <v>93</v>
       </c>
-      <c r="P3">
+      <c r="N3">
         <f>SUM(F3:J3)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45587</v>
       </c>
@@ -621,12 +622,12 @@
       <c r="M4">
         <v>77</v>
       </c>
-      <c r="P4">
-        <f t="shared" ref="P4:P55" si="0">SUM(F4:J4)</f>
+      <c r="N4">
+        <f t="shared" ref="N4:N67" si="0">SUM(F4:J4)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45587</v>
       </c>
@@ -660,12 +661,12 @@
       <c r="M5">
         <v>63</v>
       </c>
-      <c r="P5">
+      <c r="N5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45587</v>
       </c>
@@ -699,12 +700,12 @@
       <c r="M6">
         <v>71</v>
       </c>
-      <c r="P6">
+      <c r="N6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45587</v>
       </c>
@@ -738,12 +739,12 @@
       <c r="M7">
         <v>59</v>
       </c>
-      <c r="P7">
+      <c r="N7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45587</v>
       </c>
@@ -780,12 +781,16 @@
       <c r="M8">
         <v>28</v>
       </c>
-      <c r="P8">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="S8">
+        <f>SUM(F3:F11)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45587</v>
       </c>
@@ -822,12 +827,16 @@
       <c r="M9">
         <v>40</v>
       </c>
-      <c r="P9">
+      <c r="N9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S9">
+        <f>SUM(F3:F21)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45587</v>
       </c>
@@ -864,12 +873,16 @@
       <c r="M10">
         <v>73</v>
       </c>
-      <c r="P10">
+      <c r="N10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S10">
+        <f>SUM(F3:F31)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45595</v>
       </c>
@@ -906,12 +919,16 @@
       <c r="M11">
         <v>68</v>
       </c>
-      <c r="P11">
+      <c r="N11">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S11">
+        <f>SUM(F3:F41)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45588</v>
       </c>
@@ -948,12 +965,16 @@
       <c r="M12">
         <v>73</v>
       </c>
-      <c r="P12">
+      <c r="N12">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S12">
+        <f>SUM(F3:F51)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45588</v>
       </c>
@@ -990,12 +1011,16 @@
       <c r="M13">
         <v>51</v>
       </c>
-      <c r="P13">
+      <c r="N13">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S13">
+        <f>SUM(F3:F61)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45588</v>
       </c>
@@ -1032,12 +1057,16 @@
       <c r="M14">
         <v>61</v>
       </c>
-      <c r="P14">
+      <c r="N14">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S14">
+        <f>SUM(F3:F71)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45588</v>
       </c>
@@ -1074,12 +1103,16 @@
       <c r="M15">
         <v>66</v>
       </c>
-      <c r="P15">
+      <c r="N15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S15">
+        <f>SUM(F3:F81)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45588</v>
       </c>
@@ -1116,12 +1149,12 @@
       <c r="M16">
         <v>83</v>
       </c>
-      <c r="P16">
+      <c r="N16">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45588</v>
       </c>
@@ -1158,12 +1191,12 @@
       <c r="M17">
         <v>53</v>
       </c>
-      <c r="P17">
+      <c r="N17">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45588</v>
       </c>
@@ -1200,12 +1233,12 @@
       <c r="M18">
         <v>91</v>
       </c>
-      <c r="P18">
+      <c r="N18">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45588</v>
       </c>
@@ -1242,12 +1275,12 @@
       <c r="M19">
         <v>83</v>
       </c>
-      <c r="P19">
+      <c r="N19">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45588</v>
       </c>
@@ -1284,12 +1317,12 @@
       <c r="M20">
         <v>73</v>
       </c>
-      <c r="P20">
+      <c r="N20">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45588</v>
       </c>
@@ -1326,12 +1359,12 @@
       <c r="M21">
         <v>91</v>
       </c>
-      <c r="P21">
+      <c r="N21">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45588</v>
       </c>
@@ -1368,12 +1401,12 @@
       <c r="M22">
         <v>93</v>
       </c>
-      <c r="P22">
+      <c r="N22">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45588</v>
       </c>
@@ -1410,12 +1443,12 @@
       <c r="M23">
         <v>102</v>
       </c>
-      <c r="P23">
+      <c r="N23">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45588</v>
       </c>
@@ -1452,12 +1485,12 @@
       <c r="M24">
         <v>88</v>
       </c>
-      <c r="P24">
+      <c r="N24">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45595</v>
       </c>
@@ -1494,12 +1527,12 @@
       <c r="M25">
         <v>83</v>
       </c>
-      <c r="P25">
+      <c r="N25">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45595</v>
       </c>
@@ -1536,12 +1569,12 @@
       <c r="M26">
         <v>54</v>
       </c>
-      <c r="P26">
+      <c r="N26">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45595</v>
       </c>
@@ -1578,12 +1611,12 @@
       <c r="M27">
         <v>87</v>
       </c>
-      <c r="P27">
+      <c r="N27">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45588</v>
       </c>
@@ -1620,12 +1653,12 @@
       <c r="M28">
         <v>60</v>
       </c>
-      <c r="P28">
+      <c r="N28">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45588</v>
       </c>
@@ -1662,12 +1695,12 @@
       <c r="M29">
         <v>102</v>
       </c>
-      <c r="P29">
+      <c r="N29">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45588</v>
       </c>
@@ -1704,12 +1737,12 @@
       <c r="M30">
         <v>100</v>
       </c>
-      <c r="P30">
+      <c r="N30">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45588</v>
       </c>
@@ -1746,12 +1779,12 @@
       <c r="M31">
         <v>102</v>
       </c>
-      <c r="P31">
+      <c r="N31">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45588</v>
       </c>
@@ -1785,12 +1818,12 @@
       <c r="M32">
         <v>95</v>
       </c>
-      <c r="P32">
+      <c r="N32">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45588</v>
       </c>
@@ -1824,12 +1857,12 @@
       <c r="M33">
         <v>104</v>
       </c>
-      <c r="P33">
+      <c r="N33">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45593</v>
       </c>
@@ -1863,15 +1896,19 @@
       <c r="K34">
         <v>3</v>
       </c>
+      <c r="L34">
+        <f t="shared" ref="L34" si="1">(M34-K34-10*J34-6*I34-8*H34-4*G34-2*F34)</f>
+        <v>11</v>
+      </c>
       <c r="M34">
         <v>62</v>
       </c>
-      <c r="P34">
+      <c r="N34">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>45593</v>
       </c>
@@ -1906,18 +1943,18 @@
         <v>15</v>
       </c>
       <c r="L35">
-        <f t="shared" ref="L35:L77" si="1">(M35-K35-10*J35-6*I35-8*H35-4*G35-2*F35)</f>
+        <f t="shared" ref="L35:L77" si="2">(M35-K35-10*J35-6*I35-8*H35-4*G35-2*F35)</f>
         <v>13</v>
       </c>
       <c r="M35">
         <v>98</v>
       </c>
-      <c r="P35">
+      <c r="N35">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>45593</v>
       </c>
@@ -1952,18 +1989,18 @@
         <v>15</v>
       </c>
       <c r="L36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="M36">
         <v>122</v>
       </c>
-      <c r="P36">
+      <c r="N36">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>45594</v>
       </c>
@@ -1998,18 +2035,18 @@
         <v>15</v>
       </c>
       <c r="L37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="M37">
         <v>114</v>
       </c>
-      <c r="P37">
+      <c r="N37">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>45594</v>
       </c>
@@ -2044,18 +2081,18 @@
         <v>15</v>
       </c>
       <c r="L38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="M38">
         <v>114</v>
       </c>
-      <c r="P38">
+      <c r="N38">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>45594</v>
       </c>
@@ -2090,18 +2127,18 @@
         <v>3</v>
       </c>
       <c r="L39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="M39">
         <v>86</v>
       </c>
-      <c r="P39">
+      <c r="N39">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>45594</v>
       </c>
@@ -2136,18 +2173,18 @@
         <v>15</v>
       </c>
       <c r="L40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="M40">
         <v>47</v>
       </c>
-      <c r="P40">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>45594</v>
       </c>
@@ -2182,18 +2219,18 @@
         <v>15</v>
       </c>
       <c r="L41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="M41">
         <v>134</v>
       </c>
-      <c r="P41">
+      <c r="N41">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>45594</v>
       </c>
@@ -2225,18 +2262,18 @@
         <v>3</v>
       </c>
       <c r="L42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="M42">
         <v>50</v>
       </c>
-      <c r="P42">
+      <c r="N42">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>45594</v>
       </c>
@@ -2271,18 +2308,18 @@
         <v>15</v>
       </c>
       <c r="L43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="M43">
         <v>90</v>
       </c>
-      <c r="P43">
+      <c r="N43">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45595</v>
       </c>
@@ -2317,18 +2354,18 @@
         <v>15</v>
       </c>
       <c r="L44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="M44">
         <v>110</v>
       </c>
-      <c r="P44">
+      <c r="N44">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>45595</v>
       </c>
@@ -2363,18 +2400,18 @@
         <v>15</v>
       </c>
       <c r="L45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="M45">
         <v>102</v>
       </c>
-      <c r="P45">
+      <c r="N45">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45595</v>
       </c>
@@ -2409,18 +2446,18 @@
         <v>15</v>
       </c>
       <c r="L46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="M46">
         <v>102</v>
       </c>
-      <c r="P46">
+      <c r="N46">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45595</v>
       </c>
@@ -2445,12 +2482,12 @@
       <c r="M47">
         <v>103</v>
       </c>
-      <c r="P47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45595</v>
       </c>
@@ -2475,12 +2512,12 @@
       <c r="M48">
         <v>94</v>
       </c>
-      <c r="P48">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45595</v>
       </c>
@@ -2515,18 +2552,18 @@
         <v>15</v>
       </c>
       <c r="L49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="M49">
         <v>83</v>
       </c>
-      <c r="P49">
+      <c r="N49">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>45595</v>
       </c>
@@ -2561,18 +2598,18 @@
         <v>3</v>
       </c>
       <c r="L50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="M50">
         <v>86</v>
       </c>
-      <c r="P50">
+      <c r="N50">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>45595</v>
       </c>
@@ -2607,18 +2644,18 @@
         <v>3</v>
       </c>
       <c r="L51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="M51">
         <v>56</v>
       </c>
-      <c r="P51">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N51">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>45595</v>
       </c>
@@ -2653,18 +2690,18 @@
         <v>3</v>
       </c>
       <c r="L52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="M52">
         <v>81</v>
       </c>
-      <c r="P52">
+      <c r="N52">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>45595</v>
       </c>
@@ -2699,18 +2736,18 @@
         <v>3</v>
       </c>
       <c r="L53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="M53">
         <v>46</v>
       </c>
-      <c r="P53">
+      <c r="N53">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>45595</v>
       </c>
@@ -2745,18 +2782,18 @@
         <v>3</v>
       </c>
       <c r="L54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="M54">
         <v>68</v>
       </c>
-      <c r="P54">
+      <c r="N54">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>45595</v>
       </c>
@@ -2785,18 +2822,18 @@
         <v>15</v>
       </c>
       <c r="L55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="M55">
         <v>122</v>
       </c>
-      <c r="P55">
+      <c r="N55">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>45612</v>
       </c>
@@ -2831,21 +2868,21 @@
         <v>15</v>
       </c>
       <c r="L56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="M56">
         <v>88</v>
       </c>
-      <c r="P56">
-        <f t="shared" ref="P56:P63" si="2">SUM(F56:J56)</f>
+      <c r="N56">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="Q56" t="s">
+      <c r="O56" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>45612</v>
       </c>
@@ -2880,21 +2917,21 @@
         <v>15</v>
       </c>
       <c r="L57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="M57">
         <v>118</v>
       </c>
-      <c r="P57">
-        <f t="shared" si="2"/>
+      <c r="N57">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="Q57" t="s">
+      <c r="O57" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>45612</v>
       </c>
@@ -2929,21 +2966,21 @@
         <v>15</v>
       </c>
       <c r="L58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="M58">
         <v>95</v>
       </c>
-      <c r="P58">
-        <f t="shared" si="2"/>
+      <c r="N58">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="Q58" t="s">
+      <c r="O58" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>45612</v>
       </c>
@@ -2975,21 +3012,21 @@
         <v>15</v>
       </c>
       <c r="L59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="M59">
         <v>127</v>
       </c>
-      <c r="P59">
-        <f t="shared" si="2"/>
+      <c r="N59">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="Q59" t="s">
+      <c r="O59" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>45612</v>
       </c>
@@ -3021,21 +3058,21 @@
         <v>15</v>
       </c>
       <c r="L60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="M60">
         <v>131</v>
       </c>
-      <c r="P60">
-        <f t="shared" si="2"/>
+      <c r="N60">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="Q60" t="s">
+      <c r="O60" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>45612</v>
       </c>
@@ -3067,21 +3104,21 @@
         <v>15</v>
       </c>
       <c r="L61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="M61">
         <v>97</v>
       </c>
-      <c r="P61">
-        <f t="shared" si="2"/>
+      <c r="N61">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="Q61" t="s">
+      <c r="O61" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>45612</v>
       </c>
@@ -3113,18 +3150,21 @@
         <v>15</v>
       </c>
       <c r="L62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="M62">
         <v>129</v>
       </c>
-      <c r="P62">
-        <f t="shared" si="2"/>
+      <c r="N62">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O62" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>45612</v>
       </c>
@@ -3156,18 +3196,21 @@
         <v>15</v>
       </c>
       <c r="L63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="M63">
         <v>129</v>
       </c>
-      <c r="P63">
-        <f t="shared" si="2"/>
+      <c r="N63">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O63" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>45615</v>
       </c>
@@ -3202,18 +3245,18 @@
         <v>15</v>
       </c>
       <c r="L64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="M64">
         <v>139</v>
       </c>
-      <c r="P64">
-        <f>SUM(F64:J64)</f>
+      <c r="N64">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>45615</v>
       </c>
@@ -3248,18 +3291,18 @@
         <v>3</v>
       </c>
       <c r="L65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="M65">
         <v>111</v>
       </c>
-      <c r="P65">
-        <f>SUM(F65:J65)</f>
+      <c r="N65">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>45615</v>
       </c>
@@ -3294,18 +3337,18 @@
         <v>3</v>
       </c>
       <c r="L66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="M66">
         <v>111</v>
       </c>
-      <c r="P66">
-        <f>SUM(F66:J66)</f>
+      <c r="N66">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>45615</v>
       </c>
@@ -3340,18 +3383,18 @@
         <v>3</v>
       </c>
       <c r="L67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="M67">
         <v>127</v>
       </c>
-      <c r="P67">
-        <f t="shared" ref="P67:P77" si="3">SUM(F67:J67)</f>
+      <c r="N67">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>45615</v>
       </c>
@@ -3386,377 +3429,377 @@
         <v>15</v>
       </c>
       <c r="L68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="M68">
         <v>118</v>
       </c>
-      <c r="P68">
+      <c r="N68">
+        <f t="shared" ref="N68:N77" si="3">SUM(F68:J68)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>45615</v>
+      </c>
+      <c r="B69" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1</v>
+      </c>
+      <c r="D69" t="s">
+        <v>23</v>
+      </c>
+      <c r="E69" t="s">
+        <v>16</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>4</v>
+      </c>
+      <c r="K69">
+        <v>15</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="M69">
+        <v>88</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>45615</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1</v>
+      </c>
+      <c r="D70" t="s">
+        <v>17</v>
+      </c>
+      <c r="E70" t="s">
+        <v>16</v>
+      </c>
+      <c r="F70">
+        <v>1</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>5</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="K70">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M70">
+        <v>72</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>45615</v>
+      </c>
+      <c r="B71" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" t="s">
+        <v>23</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>21</v>
+      </c>
+      <c r="F71">
+        <v>1</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>7</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="K71">
+        <v>15</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="M71">
+        <v>111</v>
+      </c>
+      <c r="N71">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>45616</v>
+      </c>
+      <c r="B72" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" t="s">
+        <v>20</v>
+      </c>
+      <c r="E72" t="s">
+        <v>16</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>5</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>3</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="M72">
+        <v>59</v>
+      </c>
+      <c r="N72">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>45616</v>
+      </c>
+      <c r="B73" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" t="s">
+        <v>20</v>
+      </c>
+      <c r="E73" t="s">
+        <v>16</v>
+      </c>
+      <c r="F73">
+        <v>1</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>8</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73">
+        <v>15</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="M73">
+        <v>105</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>45616</v>
+      </c>
+      <c r="B74" t="s">
+        <v>17</v>
+      </c>
+      <c r="C74" t="s">
+        <v>23</v>
+      </c>
+      <c r="D74" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" t="s">
+        <v>21</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>8</v>
+      </c>
+      <c r="K74">
+        <v>3</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="M74">
+        <v>116</v>
+      </c>
+      <c r="N74">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <v>45615</v>
-      </c>
-      <c r="B69" t="s">
-        <v>18</v>
-      </c>
-      <c r="C69" t="s">
-        <v>1</v>
-      </c>
-      <c r="D69" t="s">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>45616</v>
+      </c>
+      <c r="B75" t="s">
+        <v>17</v>
+      </c>
+      <c r="C75" t="s">
         <v>23</v>
       </c>
-      <c r="E69" t="s">
-        <v>16</v>
-      </c>
-      <c r="F69">
-        <v>0</v>
-      </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-      <c r="H69">
-        <v>0</v>
-      </c>
-      <c r="I69">
-        <v>0</v>
-      </c>
-      <c r="J69">
-        <v>4</v>
-      </c>
-      <c r="K69">
-        <v>15</v>
-      </c>
-      <c r="L69">
-        <f t="shared" si="1"/>
+      <c r="D75" t="s">
+        <v>19</v>
+      </c>
+      <c r="E75" t="s">
+        <v>21</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>7</v>
+      </c>
+      <c r="K75">
+        <v>3</v>
+      </c>
+      <c r="L75">
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="M69">
-        <v>88</v>
-      </c>
-      <c r="P69">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
-        <v>45615</v>
-      </c>
-      <c r="B70" t="s">
-        <v>18</v>
-      </c>
-      <c r="C70" t="s">
-        <v>1</v>
-      </c>
-      <c r="D70" t="s">
-        <v>17</v>
-      </c>
-      <c r="E70" t="s">
-        <v>16</v>
-      </c>
-      <c r="F70">
-        <v>1</v>
-      </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
-      <c r="H70">
-        <v>5</v>
-      </c>
-      <c r="I70">
-        <v>0</v>
-      </c>
-      <c r="J70">
-        <v>1</v>
-      </c>
-      <c r="K70">
-        <v>0</v>
-      </c>
-      <c r="L70">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="M70">
-        <v>72</v>
-      </c>
-      <c r="P70">
+      <c r="M75">
+        <v>106</v>
+      </c>
+      <c r="N75">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <v>45615</v>
-      </c>
-      <c r="B71" t="s">
-        <v>17</v>
-      </c>
-      <c r="C71" t="s">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>45616</v>
+      </c>
+      <c r="B76" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" t="s">
         <v>23</v>
       </c>
-      <c r="D71" t="s">
-        <v>1</v>
-      </c>
-      <c r="E71" t="s">
-        <v>21</v>
-      </c>
-      <c r="F71">
-        <v>1</v>
-      </c>
-      <c r="G71">
-        <v>0</v>
-      </c>
-      <c r="H71">
+      <c r="E76" t="s">
+        <v>16</v>
+      </c>
+      <c r="F76">
+        <v>1</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
         <v>7</v>
       </c>
-      <c r="I71">
-        <v>0</v>
-      </c>
-      <c r="J71">
-        <v>1</v>
-      </c>
-      <c r="K71">
-        <v>15</v>
-      </c>
-      <c r="L71">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="M71">
-        <v>111</v>
-      </c>
-      <c r="P71">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>45616</v>
-      </c>
-      <c r="B72" t="s">
-        <v>18</v>
-      </c>
-      <c r="C72" t="s">
-        <v>20</v>
-      </c>
-      <c r="E72" t="s">
-        <v>16</v>
-      </c>
-      <c r="F72">
-        <v>0</v>
-      </c>
-      <c r="G72">
-        <v>0</v>
-      </c>
-      <c r="H72">
-        <v>5</v>
-      </c>
-      <c r="I72">
-        <v>0</v>
-      </c>
-      <c r="J72">
-        <v>0</v>
-      </c>
-      <c r="K72">
-        <v>3</v>
-      </c>
-      <c r="L72">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="M72">
-        <v>59</v>
-      </c>
-      <c r="P72">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
-        <v>45616</v>
-      </c>
-      <c r="B73" t="s">
-        <v>17</v>
-      </c>
-      <c r="C73" t="s">
-        <v>20</v>
-      </c>
-      <c r="E73" t="s">
-        <v>16</v>
-      </c>
-      <c r="F73">
-        <v>1</v>
-      </c>
-      <c r="G73">
-        <v>0</v>
-      </c>
-      <c r="H73">
-        <v>8</v>
-      </c>
-      <c r="I73">
-        <v>0</v>
-      </c>
-      <c r="J73">
-        <v>0</v>
-      </c>
-      <c r="K73">
-        <v>15</v>
-      </c>
-      <c r="L73">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="M73">
-        <v>105</v>
-      </c>
-      <c r="P73">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>45616</v>
-      </c>
-      <c r="B74" t="s">
-        <v>17</v>
-      </c>
-      <c r="C74" t="s">
-        <v>23</v>
-      </c>
-      <c r="D74" t="s">
-        <v>19</v>
-      </c>
-      <c r="E74" t="s">
-        <v>21</v>
-      </c>
-      <c r="F74">
-        <v>0</v>
-      </c>
-      <c r="G74">
-        <v>0</v>
-      </c>
-      <c r="H74">
-        <v>0</v>
-      </c>
-      <c r="I74">
-        <v>0</v>
-      </c>
-      <c r="J74">
-        <v>8</v>
-      </c>
-      <c r="K74">
-        <v>3</v>
-      </c>
-      <c r="L74">
-        <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="M74">
-        <v>116</v>
-      </c>
-      <c r="P74">
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+      <c r="K76">
+        <v>15</v>
+      </c>
+      <c r="L76">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="M76">
+        <v>89</v>
+      </c>
+      <c r="N76">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
-        <v>45616</v>
-      </c>
-      <c r="B75" t="s">
-        <v>17</v>
-      </c>
-      <c r="C75" t="s">
-        <v>23</v>
-      </c>
-      <c r="D75" t="s">
-        <v>19</v>
-      </c>
-      <c r="E75" t="s">
-        <v>21</v>
-      </c>
-      <c r="F75">
-        <v>0</v>
-      </c>
-      <c r="G75">
-        <v>0</v>
-      </c>
-      <c r="H75">
-        <v>0</v>
-      </c>
-      <c r="I75">
-        <v>0</v>
-      </c>
-      <c r="J75">
-        <v>7</v>
-      </c>
-      <c r="K75">
-        <v>3</v>
-      </c>
-      <c r="L75">
-        <f t="shared" si="1"/>
-        <v>33</v>
-      </c>
-      <c r="M75">
-        <v>106</v>
-      </c>
-      <c r="P75">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>45616</v>
-      </c>
-      <c r="B76" t="s">
-        <v>15</v>
-      </c>
-      <c r="C76" t="s">
-        <v>23</v>
-      </c>
-      <c r="E76" t="s">
-        <v>16</v>
-      </c>
-      <c r="F76">
-        <v>1</v>
-      </c>
-      <c r="G76">
-        <v>0</v>
-      </c>
-      <c r="H76">
-        <v>7</v>
-      </c>
-      <c r="I76">
-        <v>0</v>
-      </c>
-      <c r="J76">
-        <v>0</v>
-      </c>
-      <c r="K76">
-        <v>15</v>
-      </c>
-      <c r="L76">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="M76">
-        <v>89</v>
-      </c>
-      <c r="P76">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>45616</v>
       </c>
@@ -3791,13 +3834,13 @@
         <v>3</v>
       </c>
       <c r="L77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="M77">
         <v>116</v>
       </c>
-      <c r="P77">
+      <c r="N77">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Oh my gosh I didn't ruin it
It's much harder to tell what data is where but it is condensed in nice little arrays so that's better? Right?
</commit_message>
<xml_diff>
--- a/FTC Stats 2024/Red Team Data.xlsx
+++ b/FTC Stats 2024/Red Team Data.xlsx
@@ -4621,7 +4621,7 @@
         <v>32</v>
       </c>
       <c r="C6" t="n" s="0">
-        <v>3.337855339056111</v>
+        <v>3.3378553390561114</v>
       </c>
       <c r="D6" t="n" s="0">
         <v>2.6005596114695426</v>
@@ -4679,7 +4679,7 @@
         <v>34</v>
       </c>
       <c r="C8" t="n" s="0">
-        <v>3.9450959176205354</v>
+        <v>3.945095917620536</v>
       </c>
       <c r="D8" t="n" s="0">
         <v>2.259189049226963</v>
@@ -4708,10 +4708,10 @@
         <v>12</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>13.85269443923982</v>
+        <v>13.852694439239823</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>3.5286479959569395</v>
+        <v>3.52864799595694</v>
       </c>
       <c r="E9" t="e" s="0">
         <v>#NUM!</v>
@@ -4737,10 +4737,10 @@
         <v>13</v>
       </c>
       <c r="C10" t="n" s="0">
-        <v>19.525495872641763</v>
+        <v>19.52549587264176</v>
       </c>
       <c r="D10" t="n" s="0">
-        <v>9.447201847542297</v>
+        <v>9.447201847542296</v>
       </c>
       <c r="E10" t="e" s="0">
         <v>#NUM!</v>
@@ -4766,10 +4766,10 @@
         <v>14</v>
       </c>
       <c r="C11" t="n" s="0">
-        <v>96.70962881243814</v>
+        <v>96.70962881243815</v>
       </c>
       <c r="D11" t="n" s="0">
-        <v>24.564634221408525</v>
+        <v>24.56463422140853</v>
       </c>
       <c r="E11" t="e" s="0">
         <v>#NUM!</v>
@@ -4795,10 +4795,10 @@
         <v>35</v>
       </c>
       <c r="C12" t="n" s="0">
-        <v>80.95543722370374</v>
+        <v>80.95543722370375</v>
       </c>
       <c r="D12" t="n" s="0">
-        <v>14.367132670937748</v>
+        <v>14.36713267093775</v>
       </c>
       <c r="E12" t="e" s="0">
         <v>#NUM!</v>
@@ -4824,10 +4824,10 @@
         <v>26</v>
       </c>
       <c r="C13" t="n" s="0">
-        <v>7.490017951633039</v>
+        <v>7.490017951633041</v>
       </c>
       <c r="D13" t="n" s="0">
-        <v>1.5760668339441335</v>
+        <v>1.576066833944134</v>
       </c>
       <c r="E13" t="e" s="0">
         <v>#NUM!</v>
@@ -4882,10 +4882,10 @@
         <v>37</v>
       </c>
       <c r="C15" t="n" s="0">
-        <v>1.3223693668153624</v>
+        <v>1.3223693668153627</v>
       </c>
       <c r="D15" t="n" s="0">
-        <v>1.105496988964681</v>
+        <v>1.1054969889646813</v>
       </c>
       <c r="E15" t="e" s="0">
         <v>#NUM!</v>
@@ -4914,7 +4914,7 @@
         <v>7.388179804922011</v>
       </c>
       <c r="D16" t="n" s="0">
-        <v>0.7909968703444609</v>
+        <v>0.790996870344461</v>
       </c>
       <c r="E16" t="e" s="0">
         <v>#NUM!</v>
@@ -4940,10 +4940,10 @@
         <v>39</v>
       </c>
       <c r="C17" t="n" s="0">
-        <v>3.5365739531004863</v>
+        <v>3.5365739531004867</v>
       </c>
       <c r="D17" t="n" s="0">
-        <v>1.6018091585617096</v>
+        <v>1.6018091585617098</v>
       </c>
       <c r="E17" t="e" s="0">
         <v>#NUM!</v>
@@ -5049,16 +5049,16 @@
         <v>#NUM!</v>
       </c>
       <c r="G4" t="n" s="0">
-        <v>0.6735813004305905</v>
+        <v>0.6735813004305907</v>
       </c>
       <c r="H4" t="n" s="0">
-        <v>0.8456588313535615</v>
+        <v>0.8456588313535617</v>
       </c>
       <c r="I4" t="n" s="0">
         <v>0.19226051951249634</v>
       </c>
       <c r="J4" t="n" s="0">
-        <v>0.3940766577066972</v>
+        <v>0.39407665770669714</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -5078,7 +5078,7 @@
         <v>#NUM!</v>
       </c>
       <c r="G5" t="n" s="0">
-        <v>0.07468586391668589</v>
+        <v>0.07468586391668591</v>
       </c>
       <c r="H5" t="n" s="0">
         <v>0.2628837873428184</v>
@@ -5107,16 +5107,16 @@
         <v>#NUM!</v>
       </c>
       <c r="G6" t="n" s="0">
-        <v>5.153181721188944</v>
+        <v>5.153181721188946</v>
       </c>
       <c r="H6" t="n" s="0">
-        <v>2.965763796109717</v>
+        <v>2.9657637961097176</v>
       </c>
       <c r="I6" t="n" s="0">
         <v>3.019961947556307</v>
       </c>
       <c r="J6" t="n" s="0">
-        <v>2.5683350690171944</v>
+        <v>2.568335069017194</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -5136,7 +5136,7 @@
         <v>#NUM!</v>
       </c>
       <c r="G7" t="n" s="0">
-        <v>0.022034646451089244</v>
+        <v>0.022034646451089254</v>
       </c>
       <c r="H7" t="n" s="0">
         <v>0.1467961879847864</v>
@@ -5165,13 +5165,13 @@
         <v>#NUM!</v>
       </c>
       <c r="G8" t="n" s="0">
-        <v>1.7319910690385054</v>
+        <v>1.7319910690385059</v>
       </c>
       <c r="H8" t="n" s="0">
-        <v>1.9762459072140128</v>
+        <v>1.976245907214013</v>
       </c>
       <c r="I8" t="n" s="0">
-        <v>3.268428831712438</v>
+        <v>3.2684288317124373</v>
       </c>
       <c r="J8" t="n" s="0">
         <v>2.296735964704708</v>
@@ -5194,16 +5194,16 @@
         <v>#NUM!</v>
       </c>
       <c r="G9" t="n" s="0">
-        <v>10.674686250247152</v>
+        <v>10.674686250247156</v>
       </c>
       <c r="H9" t="n" s="0">
-        <v>6.158743532274594</v>
+        <v>6.158743532274595</v>
       </c>
       <c r="I9" t="n" s="0">
-        <v>11.074941819524845</v>
+        <v>11.074941819524849</v>
       </c>
       <c r="J9" t="n" s="0">
-        <v>5.629797194001479</v>
+        <v>5.629797194001478</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -5223,10 +5223,10 @@
         <v>#NUM!</v>
       </c>
       <c r="G10" t="n" s="0">
-        <v>22.620673088122903</v>
+        <v>22.6206730881229</v>
       </c>
       <c r="H10" t="n" s="0">
-        <v>7.3157130399153045</v>
+        <v>7.315713039915304</v>
       </c>
       <c r="I10" t="n" s="0">
         <v>11.0</v>
@@ -5252,10 +5252,10 @@
         <v>#NUM!</v>
       </c>
       <c r="G11" t="n" s="0">
-        <v>89.93162542681408</v>
+        <v>89.9316254268141</v>
       </c>
       <c r="H11" t="n" s="0">
-        <v>23.601701336253246</v>
+        <v>23.601701336253253</v>
       </c>
       <c r="I11" t="n" s="0">
         <v>71.03624441708733</v>
@@ -5281,7 +5281,7 @@
         <v>#NUM!</v>
       </c>
       <c r="G12" t="n" s="0">
-        <v>72.49576915180586</v>
+        <v>72.49576915180589</v>
       </c>
       <c r="H12" t="n" s="0">
         <v>20.18936739255017</v>
@@ -5290,7 +5290,7 @@
         <v>70.41831247076213</v>
       </c>
       <c r="J12" t="n" s="0">
-        <v>15.605963532386655</v>
+        <v>15.605963532386653</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -5310,16 +5310,16 @@
         <v>#NUM!</v>
       </c>
       <c r="G13" t="n" s="0">
-        <v>7.655474601025813</v>
+        <v>7.655474601025817</v>
       </c>
       <c r="H13" t="n" s="0">
-        <v>2.5573581002764287</v>
+        <v>2.557358100276429</v>
       </c>
       <c r="I13" t="n" s="0">
         <v>6.4806512987812415</v>
       </c>
       <c r="J13" t="n" s="0">
-        <v>1.5989846346701093</v>
+        <v>1.5989846346701098</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -5339,13 +5339,13 @@
         <v>#NUM!</v>
       </c>
       <c r="G14" t="n" s="0">
-        <v>0.07468586391668589</v>
+        <v>0.07468586391668591</v>
       </c>
       <c r="H14" t="n" s="0">
         <v>0.2628837873428184</v>
       </c>
       <c r="I14" t="n" s="0">
-        <v>0.13482766219376646</v>
+        <v>0.1348276621937665</v>
       </c>
       <c r="J14" t="n" s="0">
         <v>0.3415394028529213</v>
@@ -5368,10 +5368,10 @@
         <v>#NUM!</v>
       </c>
       <c r="G15" t="n" s="0">
-        <v>1.4211025602698637</v>
+        <v>1.421102560269864</v>
       </c>
       <c r="H15" t="n" s="0">
-        <v>1.029179138598117</v>
+        <v>1.0291791385981173</v>
       </c>
       <c r="I15" t="n" s="0">
         <v>0.0</v>
@@ -5397,10 +5397,10 @@
         <v>#NUM!</v>
       </c>
       <c r="G16" t="n" s="0">
-        <v>6.482291431266711</v>
+        <v>6.48229143126671</v>
       </c>
       <c r="H16" t="n" s="0">
-        <v>1.5427728873241637</v>
+        <v>1.542772887324164</v>
       </c>
       <c r="I16" t="n" s="0">
         <v>5.0</v>
@@ -5426,10 +5426,10 @@
         <v>#NUM!</v>
       </c>
       <c r="G17" t="n" s="0">
-        <v>2.0907820056187383</v>
+        <v>2.0907820056187387</v>
       </c>
       <c r="H17" t="n" s="0">
-        <v>1.8373210007542564</v>
+        <v>1.8373210007542566</v>
       </c>
       <c r="I17" t="e" s="0">
         <v>#NUM!</v>
@@ -5517,16 +5517,16 @@
         <v>#NUM!</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>0.2333926440968066</v>
+        <v>0.2333926440968067</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>0.42298997361439666</v>
+        <v>0.4229899736143968</v>
       </c>
       <c r="G4" t="n" s="0">
-        <v>0.1377850658040971</v>
+        <v>0.13778506580409716</v>
       </c>
       <c r="H4" t="n" s="0">
-        <v>0.3920880939201407</v>
+        <v>0.39208809392014077</v>
       </c>
       <c r="I4" t="n" s="0">
         <v>0.0</v>
@@ -5546,16 +5546,16 @@
         <v>#NUM!</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>0.09335705763872264</v>
+        <v>0.09335705763872268</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>0.4218987734830305</v>
+        <v>0.4218987734830306</v>
       </c>
       <c r="G5" t="n" s="0">
-        <v>0.018689011592432147</v>
+        <v>0.018689011592432154</v>
       </c>
       <c r="H5" t="n" s="0">
-        <v>0.1354242682761479</v>
+        <v>0.13542426827614798</v>
       </c>
       <c r="I5" t="n" s="0">
         <v>0.0</v>
@@ -5575,16 +5575,16 @@
         <v>#NUM!</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>3.878365954253243</v>
+        <v>3.878365954253245</v>
       </c>
       <c r="F6" t="n" s="0">
-        <v>3.263836403992898</v>
+        <v>3.2638364039928986</v>
       </c>
       <c r="G6" t="n" s="0">
-        <v>3.7269448495684703</v>
+        <v>3.726944849568471</v>
       </c>
       <c r="H6" t="n" s="0">
-        <v>3.877410432465711</v>
+        <v>3.8774104324657124</v>
       </c>
       <c r="I6" t="n" s="0">
         <v>1.0</v>
@@ -5636,10 +5636,10 @@
         <v>3.6436239560743515</v>
       </c>
       <c r="F8" t="n" s="0">
-        <v>2.162500069974971</v>
+        <v>2.1625000699749712</v>
       </c>
       <c r="G8" t="n" s="0">
-        <v>4.229632258646526</v>
+        <v>4.229632258646528</v>
       </c>
       <c r="H8" t="n" s="0">
         <v>2.9563542870287494</v>
@@ -5662,13 +5662,13 @@
         <v>#NUM!</v>
       </c>
       <c r="E9" t="n" s="0">
-        <v>10.621174353116771</v>
+        <v>10.621174353116777</v>
       </c>
       <c r="F9" t="n" s="0">
-        <v>5.776832498592668</v>
+        <v>5.776832498592669</v>
       </c>
       <c r="G9" t="n" s="0">
-        <v>10.342369802774147</v>
+        <v>10.342369802774153</v>
       </c>
       <c r="H9" t="n" s="0">
         <v>5.847909311249628</v>
@@ -5691,16 +5691,16 @@
         <v>#NUM!</v>
       </c>
       <c r="E10" t="n" s="0">
-        <v>18.25</v>
+        <v>18.249999999999996</v>
       </c>
       <c r="F10" t="n" s="0">
         <v>9.256754290786809</v>
       </c>
       <c r="G10" t="n" s="0">
-        <v>26.779505302001745</v>
+        <v>26.779505302001752</v>
       </c>
       <c r="H10" t="n" s="0">
-        <v>8.14727521317455</v>
+        <v>8.147275213174552</v>
       </c>
       <c r="I10" t="e" s="0">
         <v>#NUM!</v>
@@ -5720,16 +5720,16 @@
         <v>#NUM!</v>
       </c>
       <c r="E11" t="n" s="0">
-        <v>85.37655690754117</v>
+        <v>85.3765569075412</v>
       </c>
       <c r="F11" t="n" s="0">
-        <v>20.066620388529685</v>
+        <v>20.066620388529692</v>
       </c>
       <c r="G11" t="n" s="0">
-        <v>108.6886384710755</v>
+        <v>108.68863847107554</v>
       </c>
       <c r="H11" t="n" s="0">
-        <v>21.962217488948898</v>
+        <v>21.962217488948905</v>
       </c>
       <c r="I11" t="n" s="0">
         <v>73.0</v>
@@ -5749,16 +5749,16 @@
         <v>#NUM!</v>
       </c>
       <c r="E12" t="n" s="0">
-        <v>80.60498210413174</v>
+        <v>80.60498210413178</v>
       </c>
       <c r="F12" t="n" s="0">
-        <v>21.08406493828033</v>
+        <v>21.084064938280335</v>
       </c>
       <c r="G12" t="n" s="0">
-        <v>83.59410399334533</v>
+        <v>83.59410399334537</v>
       </c>
       <c r="H12" t="n" s="0">
-        <v>15.237542342912866</v>
+        <v>15.237542342912867</v>
       </c>
       <c r="I12" t="n" s="0">
         <v>74.0</v>
@@ -5778,16 +5778,16 @@
         <v>#NUM!</v>
       </c>
       <c r="E13" t="n" s="0">
-        <v>7.848739612063124</v>
+        <v>7.8487396120631265</v>
       </c>
       <c r="F13" t="n" s="0">
-        <v>2.2086049561322665</v>
+        <v>2.208604956132267</v>
       </c>
       <c r="G13" t="n" s="0">
-        <v>8.113051185611527</v>
+        <v>8.113051185611528</v>
       </c>
       <c r="H13" t="n" s="0">
-        <v>1.8752641322499541</v>
+        <v>1.8752641322499548</v>
       </c>
       <c r="I13" t="n" s="0">
         <v>6.0</v>
@@ -5813,7 +5813,7 @@
         <v>0.0</v>
       </c>
       <c r="G14" t="n" s="0">
-        <v>0.10631481761014132</v>
+        <v>0.10631481761014133</v>
       </c>
       <c r="H14" t="n" s="0">
         <v>0.30824012906606385</v>
@@ -5836,16 +5836,16 @@
         <v>#NUM!</v>
       </c>
       <c r="E15" t="n" s="0">
-        <v>0.3747775846369749</v>
+        <v>0.3747775846369752</v>
       </c>
       <c r="F15" t="n" s="0">
-        <v>0.7308497892181607</v>
+        <v>0.730849789218161</v>
       </c>
       <c r="G15" t="n" s="0">
-        <v>2.132896387351895</v>
+        <v>2.132896387351896</v>
       </c>
       <c r="H15" t="n" s="0">
-        <v>1.0153066969089732</v>
+        <v>1.0153066969089735</v>
       </c>
       <c r="I15" t="n" s="0">
         <v>0.0</v>
@@ -5871,7 +5871,7 @@
         <v>0.0</v>
       </c>
       <c r="G16" t="n" s="0">
-        <v>7.923828465667523</v>
+        <v>7.92382846566752</v>
       </c>
       <c r="H16" t="n" s="0">
         <v>2.34687723292636</v>
@@ -5894,7 +5894,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E17" t="n" s="0">
-        <v>2.333333333333333</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="F17" t="n" s="0">
         <v>1.247219128924647</v>
@@ -5903,7 +5903,7 @@
         <v>4.114889337859332</v>
       </c>
       <c r="H17" t="n" s="0">
-        <v>1.4017378619461325</v>
+        <v>1.4017378619461323</v>
       </c>
       <c r="I17" t="e" s="0">
         <v>#NUM!</v>
@@ -5997,10 +5997,10 @@
         <v>#NUM!</v>
       </c>
       <c r="G4" t="n" s="0">
-        <v>0.027332804325900174</v>
+        <v>0.027332804325900177</v>
       </c>
       <c r="H4" t="n" s="0">
-        <v>0.1630512868197679</v>
+        <v>0.16305128681976794</v>
       </c>
       <c r="I4" t="n" s="0">
         <v>0.5</v>
@@ -6017,7 +6017,7 @@
         <v>0.20820794277877105</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>0.6107907482283716</v>
+        <v>0.6107907482283718</v>
       </c>
       <c r="E5" t="e" s="0">
         <v>#NUM!</v>
@@ -6055,7 +6055,7 @@
         <v>#NUM!</v>
       </c>
       <c r="G6" t="n" s="0">
-        <v>3.1417046601581347</v>
+        <v>3.141704660158134</v>
       </c>
       <c r="H6" t="n" s="0">
         <v>2.3649002807029644</v>
@@ -6113,13 +6113,13 @@
         <v>#NUM!</v>
       </c>
       <c r="G8" t="n" s="0">
-        <v>4.183086959193259</v>
+        <v>4.18308695919326</v>
       </c>
       <c r="H8" t="n" s="0">
         <v>1.6804555992369636</v>
       </c>
       <c r="I8" t="n" s="0">
-        <v>6.000000000000001</v>
+        <v>6.0</v>
       </c>
       <c r="J8" t="n" s="0">
         <v>1.0</v>
@@ -6130,10 +6130,10 @@
         <v>12</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>13.750752343327372</v>
+        <v>13.750752343327374</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>3.66474448937023</v>
+        <v>3.6647444893702303</v>
       </c>
       <c r="E9" t="e" s="0">
         <v>#NUM!</v>
@@ -6142,10 +6142,10 @@
         <v>#NUM!</v>
       </c>
       <c r="G9" t="n" s="0">
-        <v>9.056401077846292</v>
+        <v>9.056401077846298</v>
       </c>
       <c r="H9" t="n" s="0">
-        <v>6.087164114597723</v>
+        <v>6.087164114597725</v>
       </c>
       <c r="I9" t="n" s="0">
         <v>15.0</v>
@@ -6171,13 +6171,13 @@
         <v>#NUM!</v>
       </c>
       <c r="G10" t="n" s="0">
-        <v>24.676979217290064</v>
+        <v>24.67697921729007</v>
       </c>
       <c r="H10" t="n" s="0">
         <v>10.494134948880093</v>
       </c>
       <c r="I10" t="n" s="0">
-        <v>18.0</v>
+        <v>17.999999999999996</v>
       </c>
       <c r="J10" t="n" s="0">
         <v>5.0</v>
@@ -6188,7 +6188,7 @@
         <v>14</v>
       </c>
       <c r="C11" t="n" s="0">
-        <v>98.78481438016703</v>
+        <v>98.78481438016705</v>
       </c>
       <c r="D11" t="n" s="0">
         <v>16.325059977726763</v>
@@ -6200,13 +6200,13 @@
         <v>#NUM!</v>
       </c>
       <c r="G11" t="n" s="0">
-        <v>94.13680097223376</v>
+        <v>94.13680097223379</v>
       </c>
       <c r="H11" t="n" s="0">
         <v>22.475802232510606</v>
       </c>
       <c r="I11" t="n" s="0">
-        <v>109.99999999999999</v>
+        <v>110.0</v>
       </c>
       <c r="J11" t="n" s="0">
         <v>12.0</v>
@@ -6229,16 +6229,16 @@
         <v>#NUM!</v>
       </c>
       <c r="G12" t="n" s="0">
-        <v>76.3880613042147</v>
+        <v>76.38806130421472</v>
       </c>
       <c r="H12" t="n" s="0">
-        <v>13.962677324528489</v>
+        <v>13.96267732452849</v>
       </c>
       <c r="I12" t="n" s="0">
         <v>92.0</v>
       </c>
       <c r="J12" t="n" s="0">
-        <v>6.999999999999999</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -6246,10 +6246,10 @@
         <v>26</v>
       </c>
       <c r="C13" t="n" s="0">
-        <v>9.375376171663687</v>
+        <v>9.375376171663689</v>
       </c>
       <c r="D13" t="n" s="0">
-        <v>1.5889481652896307</v>
+        <v>1.5889481652896305</v>
       </c>
       <c r="E13" t="e" s="0">
         <v>#NUM!</v>
@@ -6258,10 +6258,10 @@
         <v>#NUM!</v>
       </c>
       <c r="G13" t="n" s="0">
-        <v>6.758827628460227</v>
+        <v>6.758827628460229</v>
       </c>
       <c r="H13" t="n" s="0">
-        <v>2.5150121180159717</v>
+        <v>2.515012118015972</v>
       </c>
       <c r="I13" t="n" s="0">
         <v>8.5</v>
@@ -6304,7 +6304,7 @@
         <v>37</v>
       </c>
       <c r="C15" t="n" s="0">
-        <v>0.33433645776983156</v>
+        <v>0.3343364577698316</v>
       </c>
       <c r="D15" t="n" s="0">
         <v>0.7462520006978774</v>
@@ -6316,13 +6316,13 @@
         <v>#NUM!</v>
       </c>
       <c r="G15" t="n" s="0">
-        <v>1.6121141158376295</v>
+        <v>1.6121141158376298</v>
       </c>
       <c r="H15" t="n" s="0">
         <v>1.3189809957315424</v>
       </c>
       <c r="I15" t="n" s="0">
-        <v>1.5000000000000002</v>
+        <v>1.5</v>
       </c>
       <c r="J15" t="n" s="0">
         <v>0.5</v>
@@ -6374,16 +6374,16 @@
         <v>#NUM!</v>
       </c>
       <c r="G17" t="n" s="0">
-        <v>3.621394472911969</v>
+        <v>3.6213944729119696</v>
       </c>
       <c r="H17" t="n" s="0">
         <v>1.8478603580782254</v>
       </c>
       <c r="I17" t="n" s="0">
-        <v>6.000000000000001</v>
+        <v>6.0</v>
       </c>
       <c r="J17" t="n" s="0">
-        <v>8.881784197001252E-16</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -6897,10 +6897,10 @@
     </row>
     <row r="4" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C4" t="n" s="0">
-        <v>0.30230939911901256</v>
+        <v>0.3023093991190126</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>0.6324945066168765</v>
+        <v>0.6324945066168763</v>
       </c>
       <c r="F4" t="s" s="0">
         <v>30</v>
@@ -6917,10 +6917,10 @@
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C5" t="n" s="0">
-        <v>0.04475560588054828</v>
+        <v>0.04475560588054829</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>0.23032607654806547</v>
+        <v>0.2303260765480654</v>
       </c>
       <c r="F5" t="s" s="0">
         <v>31</v>
@@ -6937,10 +6937,10 @@
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C6" t="n" s="0">
-        <v>4.156072076962745</v>
+        <v>4.156072076962746</v>
       </c>
       <c r="D6" t="n" s="0">
-        <v>3.4273423643591436</v>
+        <v>3.427342364359144</v>
       </c>
       <c r="F6" t="s" s="0">
         <v>32</v>
@@ -6957,10 +6957,10 @@
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C7" t="n" s="0">
-        <v>0.007726930357371098</v>
+        <v>0.0077269303573711005</v>
       </c>
       <c r="D7" t="n" s="0">
-        <v>0.08756269128243739</v>
+        <v>0.08756269128243738</v>
       </c>
       <c r="F7" t="s" s="0">
         <v>33</v>
@@ -6977,10 +6977,10 @@
     </row>
     <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8" t="n" s="0">
-        <v>3.3334213092849203</v>
+        <v>3.333421309284922</v>
       </c>
       <c r="D8" t="n" s="0">
-        <v>2.7122605002297044</v>
+        <v>2.712260500229705</v>
       </c>
       <c r="F8" t="s" s="0">
         <v>34</v>
@@ -6997,10 +6997,10 @@
     </row>
     <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" t="n" s="0">
-        <v>10.222071412082034</v>
+        <v>10.222071412082043</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>6.029334398199037</v>
+        <v>6.029334398199039</v>
       </c>
       <c r="F9" t="s" s="0">
         <v>12</v>
@@ -7017,7 +7017,7 @@
     </row>
     <row r="10" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C10" t="n" s="0">
-        <v>25.066661458261123</v>
+        <v>25.066661458261116</v>
       </c>
       <c r="D10" t="n" s="0">
         <v>8.528665201003093</v>
@@ -7037,10 +7037,10 @@
     </row>
     <row r="11" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C11" t="n" s="0">
-        <v>99.2999585007811</v>
+        <v>99.29995850078114</v>
       </c>
       <c r="D11" t="n" s="0">
-        <v>24.131048982123826</v>
+        <v>24.13104898212383</v>
       </c>
       <c r="F11" t="s" s="0">
         <v>14</v>
@@ -7057,10 +7057,10 @@
     </row>
     <row r="12" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C12" t="n" s="0">
-        <v>78.57699767580291</v>
+        <v>78.5769976758029</v>
       </c>
       <c r="D12" t="n" s="0">
-        <v>17.688989345175383</v>
+        <v>17.688989345175386</v>
       </c>
       <c r="F12" t="s" s="0">
         <v>35</v>
@@ -7077,7 +7077,7 @@
     </row>
     <row r="13" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C13" t="n" s="0">
-        <v>7.716685065096772</v>
+        <v>7.716685065096776</v>
       </c>
       <c r="D13" t="n" s="0">
         <v>2.3262358641282663</v>
@@ -7097,10 +7097,10 @@
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C14" t="n" s="0">
-        <v>0.07203166064418558</v>
+        <v>0.07203166064418559</v>
       </c>
       <c r="D14" t="n" s="0">
-        <v>0.25854032665916243</v>
+        <v>0.25854032665916254</v>
       </c>
       <c r="F14" t="s" s="0">
         <v>36</v>
@@ -7117,7 +7117,7 @@
     </row>
     <row r="15" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C15" t="n" s="0">
-        <v>1.7596860841512858</v>
+        <v>1.7596860841512862</v>
       </c>
       <c r="D15" t="n" s="0">
         <v>1.1406510768142801</v>
@@ -7137,7 +7137,7 @@
     </row>
     <row r="16" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C16" t="n" s="0">
-        <v>6.9802756259830865</v>
+        <v>6.980275625983086</v>
       </c>
       <c r="D16" t="n" s="0">
         <v>2.0430970562275377</v>
@@ -7157,10 +7157,10 @@
     </row>
     <row r="17" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C17" t="n" s="0">
-        <v>3.727451558455866</v>
+        <v>3.7274515584558654</v>
       </c>
       <c r="D17" t="n" s="0">
-        <v>1.7136988127227228</v>
+        <v>1.7136988127227226</v>
       </c>
       <c r="F17" t="s" s="0">
         <v>39</v>
@@ -7275,7 +7275,7 @@
         <v>0.21580483433267625</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>0.41137951797740535</v>
+        <v>0.4113795179774054</v>
       </c>
       <c r="E5" t="e" s="0">
         <v>#NUM!</v>
@@ -7391,7 +7391,7 @@
         <v>8.655115160030286</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>5.990079669516848</v>
+        <v>5.990079669516847</v>
       </c>
       <c r="E9" t="e" s="0">
         <v>#NUM!</v>
@@ -7420,7 +7420,7 @@
         <v>32.67414427496457</v>
       </c>
       <c r="D10" t="n" s="0">
-        <v>1.694516220508944</v>
+        <v>1.6945162205089437</v>
       </c>
       <c r="E10" t="e" s="0">
         <v>#NUM!</v>
@@ -7475,7 +7475,7 @@
         <v>35</v>
       </c>
       <c r="C12" t="n" s="0">
-        <v>83.9108456067111</v>
+        <v>83.91084560671109</v>
       </c>
       <c r="D12" t="n" s="0">
         <v>6.081653755880387</v>
@@ -7507,7 +7507,7 @@
         <v>8.735629798334596</v>
       </c>
       <c r="D13" t="n" s="0">
-        <v>0.7912573960489409</v>
+        <v>0.791257396048941</v>
       </c>
       <c r="E13" t="e" s="0">
         <v>#NUM!</v>
@@ -7562,7 +7562,7 @@
         <v>37</v>
       </c>
       <c r="C15" t="n" s="0">
-        <v>2.881050215988486</v>
+        <v>2.8810502159884863</v>
       </c>
       <c r="D15" t="n" s="0">
         <v>0.5854060991467003</v>
@@ -7723,10 +7723,10 @@
         <v>#NUM!</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>0.3838239641560619</v>
+        <v>0.38382396415606196</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>0.852111998696291</v>
+        <v>0.8521119986962911</v>
       </c>
       <c r="G4" t="e" s="0">
         <v>#NUM!</v>
@@ -7781,7 +7781,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>4.145995091308957</v>
+        <v>4.145995091308958</v>
       </c>
       <c r="F6" t="n" s="0">
         <v>3.287983165938051</v>
@@ -7793,7 +7793,7 @@
         <v>#NUM!</v>
       </c>
       <c r="I6" t="n" s="0">
-        <v>4.857658415927463</v>
+        <v>4.857658415927464</v>
       </c>
       <c r="J6" t="n" s="0">
         <v>3.558013447305554</v>
@@ -7810,7 +7810,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E7" t="n" s="0">
-        <v>0.02407412438792454</v>
+        <v>0.024074124387924542</v>
       </c>
       <c r="F7" t="n" s="0">
         <v>0.15327935582745406</v>
@@ -7839,10 +7839,10 @@
         <v>#NUM!</v>
       </c>
       <c r="E8" t="n" s="0">
-        <v>3.447752184606647</v>
+        <v>3.4477521846066463</v>
       </c>
       <c r="F8" t="n" s="0">
-        <v>2.250106547686539</v>
+        <v>2.2501065476865394</v>
       </c>
       <c r="G8" t="e" s="0">
         <v>#NUM!</v>
@@ -7883,7 +7883,7 @@
         <v>13.960294123594235</v>
       </c>
       <c r="J9" t="n" s="0">
-        <v>3.375719509591473</v>
+        <v>3.3757195095914727</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -7897,10 +7897,10 @@
         <v>#NUM!</v>
       </c>
       <c r="E10" t="n" s="0">
-        <v>26.90812404084688</v>
+        <v>26.908124040846882</v>
       </c>
       <c r="F10" t="n" s="0">
-        <v>7.109111492656764</v>
+        <v>7.109111492656765</v>
       </c>
       <c r="G10" t="e" s="0">
         <v>#NUM!</v>
@@ -7909,7 +7909,7 @@
         <v>#NUM!</v>
       </c>
       <c r="I10" t="n" s="0">
-        <v>21.94872882679837</v>
+        <v>21.948728826798373</v>
       </c>
       <c r="J10" t="n" s="0">
         <v>8.023400727729282</v>
@@ -7926,10 +7926,10 @@
         <v>#NUM!</v>
       </c>
       <c r="E11" t="n" s="0">
-        <v>103.4409782204388</v>
+        <v>103.44097822043878</v>
       </c>
       <c r="F11" t="n" s="0">
-        <v>26.56977779535065</v>
+        <v>26.569777795350653</v>
       </c>
       <c r="G11" t="e" s="0">
         <v>#NUM!</v>
@@ -7938,7 +7938,7 @@
         <v>#NUM!</v>
       </c>
       <c r="I11" t="n" s="0">
-        <v>98.78710317212344</v>
+        <v>98.78710317212345</v>
       </c>
       <c r="J11" t="n" s="0">
         <v>21.490658293119683</v>
@@ -7955,10 +7955,10 @@
         <v>#NUM!</v>
       </c>
       <c r="E12" t="n" s="0">
-        <v>79.88007749451721</v>
+        <v>79.88007749451722</v>
       </c>
       <c r="F12" t="n" s="0">
-        <v>19.862400225769825</v>
+        <v>19.86240022576982</v>
       </c>
       <c r="G12" t="e" s="0">
         <v>#NUM!</v>
@@ -7984,7 +7984,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E13" t="n" s="0">
-        <v>8.00164536445959</v>
+        <v>8.001645364459588</v>
       </c>
       <c r="F13" t="n" s="0">
         <v>2.4933169768329453</v>
@@ -7996,10 +7996,10 @@
         <v>#NUM!</v>
       </c>
       <c r="I13" t="n" s="0">
-        <v>7.685775177719099</v>
+        <v>7.685775177719098</v>
       </c>
       <c r="J13" t="n" s="0">
-        <v>2.1138078552435315</v>
+        <v>2.113807855243532</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -8045,7 +8045,7 @@
         <v>2.051024034478572</v>
       </c>
       <c r="F15" t="n" s="0">
-        <v>1.0601104888797614</v>
+        <v>1.0601104888797612</v>
       </c>
       <c r="G15" t="e" s="0">
         <v>#NUM!</v>
@@ -8054,7 +8054,7 @@
         <v>#NUM!</v>
       </c>
       <c r="I15" t="n" s="0">
-        <v>1.5330443404506504</v>
+        <v>1.5330443404506502</v>
       </c>
       <c r="J15" t="n" s="0">
         <v>0.649763329450405</v>
@@ -8071,10 +8071,10 @@
         <v>#NUM!</v>
       </c>
       <c r="E16" t="n" s="0">
-        <v>6.876283429862217</v>
+        <v>6.876283429862218</v>
       </c>
       <c r="F16" t="n" s="0">
-        <v>2.2512578499557647</v>
+        <v>2.251257849955765</v>
       </c>
       <c r="G16" t="e" s="0">
         <v>#NUM!</v>
@@ -8083,7 +8083,7 @@
         <v>#NUM!</v>
       </c>
       <c r="I16" t="n" s="0">
-        <v>6.2453309970548805</v>
+        <v>6.245330997054882</v>
       </c>
       <c r="J16" t="n" s="0">
         <v>2.256493660535427</v>
@@ -8100,7 +8100,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E17" t="n" s="0">
-        <v>3.041291642003447</v>
+        <v>3.0412916420034475</v>
       </c>
       <c r="F17" t="n" s="0">
         <v>1.8630136439445126</v>
@@ -8252,7 +8252,7 @@
         <v>3.9820076887092166</v>
       </c>
       <c r="D6" t="n" s="0">
-        <v>4.294264432694481</v>
+        <v>4.29426443269448</v>
       </c>
       <c r="E6" t="e" s="0">
         <v>#NUM!</v>
@@ -8270,7 +8270,7 @@
         <v>3.627467431762574</v>
       </c>
       <c r="J6" t="n" s="0">
-        <v>3.686869105679458</v>
+        <v>3.6868691056794574</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -8307,7 +8307,7 @@
         <v>34</v>
       </c>
       <c r="C8" t="n" s="0">
-        <v>3.861533138597799</v>
+        <v>3.8615331385977996</v>
       </c>
       <c r="D8" t="n" s="0">
         <v>3.0739538699203313</v>
@@ -8325,7 +8325,7 @@
         <v>#NUM!</v>
       </c>
       <c r="I8" t="n" s="0">
-        <v>4.651041821059261</v>
+        <v>4.65104182105926</v>
       </c>
       <c r="J8" t="n" s="0">
         <v>2.575114576863736</v>
@@ -8336,7 +8336,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>10.131460471234828</v>
+        <v>10.13146047123483</v>
       </c>
       <c r="D9" t="n" s="0">
         <v>5.892350736508567</v>
@@ -8365,7 +8365,7 @@
         <v>13</v>
       </c>
       <c r="C10" t="n" s="0">
-        <v>22.821272055065847</v>
+        <v>22.821272055065844</v>
       </c>
       <c r="D10" t="n" s="0">
         <v>8.635225440445064</v>
@@ -8383,7 +8383,7 @@
         <v>#NUM!</v>
       </c>
       <c r="I10" t="n" s="0">
-        <v>29.154692677627285</v>
+        <v>29.154692677627292</v>
       </c>
       <c r="J10" t="n" s="0">
         <v>7.89276906759154</v>
@@ -8423,7 +8423,7 @@
         <v>35</v>
       </c>
       <c r="C12" t="n" s="0">
-        <v>83.6233312141909</v>
+        <v>83.62333121419091</v>
       </c>
       <c r="D12" t="n" s="0">
         <v>11.472156991046678</v>
@@ -8528,7 +8528,7 @@
         <v>#NUM!</v>
       </c>
       <c r="I15" t="n" s="0">
-        <v>2.648483252742597</v>
+        <v>2.6484832527425968</v>
       </c>
       <c r="J15" t="n" s="0">
         <v>0.7164173945018868</v>
@@ -8542,7 +8542,7 @@
         <v>8.576621163822054</v>
       </c>
       <c r="D16" t="n" s="0">
-        <v>1.98605890798745</v>
+        <v>1.9860589079874498</v>
       </c>
       <c r="E16" t="e" s="0">
         <v>#NUM!</v>
@@ -8557,10 +8557,10 @@
         <v>#NUM!</v>
       </c>
       <c r="I16" t="n" s="0">
-        <v>7.333882770815181</v>
+        <v>7.3338827708151815</v>
       </c>
       <c r="J16" t="n" s="0">
-        <v>2.063650978668431</v>
+        <v>2.0636509786684316</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -8568,10 +8568,10 @@
         <v>39</v>
       </c>
       <c r="C17" t="n" s="0">
-        <v>5.357913345714892</v>
+        <v>5.357913345714891</v>
       </c>
       <c r="D17" t="n" s="0">
-        <v>0.6915994338654978</v>
+        <v>0.6915994338654977</v>
       </c>
       <c r="E17" t="e" s="0">
         <v>#NUM!</v>
@@ -8683,7 +8683,7 @@
         <v>#NUM!</v>
       </c>
       <c r="I4" t="n" s="0">
-        <v>0.3120229494275608</v>
+        <v>0.31202294942756076</v>
       </c>
       <c r="J4" t="n" s="0">
         <v>0.4633191432027028</v>
@@ -8694,7 +8694,7 @@
         <v>31</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>0.02456114361966217</v>
+        <v>0.024561143619662173</v>
       </c>
       <c r="D5" t="n" s="0">
         <v>0.15478337715580606</v>
@@ -8741,7 +8741,7 @@
         <v>#NUM!</v>
       </c>
       <c r="I6" t="n" s="0">
-        <v>4.680344241413412</v>
+        <v>4.680344241413413</v>
       </c>
       <c r="J6" t="n" s="0">
         <v>4.072566420155094</v>
@@ -8781,7 +8781,7 @@
         <v>34</v>
       </c>
       <c r="C8" t="n" s="0">
-        <v>3.7253654960072895</v>
+        <v>3.72536549600729</v>
       </c>
       <c r="D8" t="n" s="0">
         <v>3.190871518806903</v>
@@ -8799,7 +8799,7 @@
         <v>#NUM!</v>
       </c>
       <c r="I8" t="n" s="0">
-        <v>3.0562983425582906</v>
+        <v>3.056298342558291</v>
       </c>
       <c r="J8" t="n" s="0">
         <v>2.959601356013859</v>
@@ -8810,10 +8810,10 @@
         <v>12</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>10.103669788111711</v>
+        <v>10.103669788111713</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>6.005701110384616</v>
+        <v>6.005701110384617</v>
       </c>
       <c r="E9" t="e" s="0">
         <v>#NUM!</v>
@@ -8828,7 +8828,7 @@
         <v>#NUM!</v>
       </c>
       <c r="I9" t="n" s="0">
-        <v>6.76717382060781</v>
+        <v>6.767173820607811</v>
       </c>
       <c r="J9" t="n" s="0">
         <v>6.494506767228889</v>
@@ -8839,10 +8839,10 @@
         <v>13</v>
       </c>
       <c r="C10" t="n" s="0">
-        <v>27.96720817012324</v>
+        <v>27.967208170123243</v>
       </c>
       <c r="D10" t="n" s="0">
-        <v>6.8851281378269</v>
+        <v>6.885128137826901</v>
       </c>
       <c r="E10" t="e" s="0">
         <v>#NUM!</v>
@@ -8857,7 +8857,7 @@
         <v>#NUM!</v>
       </c>
       <c r="I10" t="n" s="0">
-        <v>23.549444512684307</v>
+        <v>23.54944451268431</v>
       </c>
       <c r="J10" t="n" s="0">
         <v>7.247399189317224</v>
@@ -8871,7 +8871,7 @@
         <v>105.94552922626735</v>
       </c>
       <c r="D11" t="n" s="0">
-        <v>24.577188109135655</v>
+        <v>24.57718810913566</v>
       </c>
       <c r="E11" t="e" s="0">
         <v>#NUM!</v>
@@ -8889,7 +8889,7 @@
         <v>98.91127496853677</v>
       </c>
       <c r="J11" t="n" s="0">
-        <v>25.858552498175122</v>
+        <v>25.85855249817512</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -8900,7 +8900,7 @@
         <v>82.73610845998617</v>
       </c>
       <c r="D12" t="n" s="0">
-        <v>16.31692659049616</v>
+        <v>16.316926590496163</v>
       </c>
       <c r="E12" t="e" s="0">
         <v>#NUM!</v>
@@ -8926,10 +8926,10 @@
         <v>26</v>
       </c>
       <c r="C13" t="n" s="0">
-        <v>8.500774540474474</v>
+        <v>8.500774540474472</v>
       </c>
       <c r="D13" t="n" s="0">
-        <v>2.1854806082281213</v>
+        <v>2.1854806082281217</v>
       </c>
       <c r="E13" t="e" s="0">
         <v>#NUM!</v>
@@ -8987,7 +8987,7 @@
         <v>1.9379418317808492</v>
       </c>
       <c r="D15" t="n" s="0">
-        <v>1.1305062232272682</v>
+        <v>1.1305062232272685</v>
       </c>
       <c r="E15" t="e" s="0">
         <v>#NUM!</v>
@@ -9002,10 +9002,10 @@
         <v>#NUM!</v>
       </c>
       <c r="I15" t="n" s="0">
-        <v>1.9923671908409732</v>
+        <v>1.992367190840973</v>
       </c>
       <c r="J15" t="n" s="0">
-        <v>0.7947455242016092</v>
+        <v>0.794745524201609</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -9013,7 +9013,7 @@
         <v>38</v>
       </c>
       <c r="C16" t="n" s="0">
-        <v>7.662202424434099</v>
+        <v>7.6622024244341</v>
       </c>
       <c r="D16" t="n" s="0">
         <v>1.9846127002345393</v>
@@ -9031,7 +9031,7 @@
         <v>#NUM!</v>
       </c>
       <c r="I16" t="n" s="0">
-        <v>7.499999999999998</v>
+        <v>7.500000000000001</v>
       </c>
       <c r="J16" t="n" s="0">
         <v>2.3303283317898176</v>
@@ -9060,7 +9060,7 @@
         <v>#NUM!</v>
       </c>
       <c r="I17" t="n" s="0">
-        <v>4.975537667427892</v>
+        <v>4.975537667427893</v>
       </c>
       <c r="J17" t="n" s="0">
         <v>2.0181151087094746</v>
@@ -9177,7 +9177,7 @@
         <v>0.08446035919668687</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>0.27807698020701654</v>
+        <v>0.2780769802070166</v>
       </c>
       <c r="G5" t="e" s="0">
         <v>#NUM!</v>
@@ -9203,10 +9203,10 @@
         <v>#NUM!</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>5.046491832163294</v>
+        <v>5.046491832163295</v>
       </c>
       <c r="F6" t="n" s="0">
-        <v>3.4647290438407774</v>
+        <v>3.464729043840778</v>
       </c>
       <c r="G6" t="e" s="0">
         <v>#NUM!</v>
@@ -9319,7 +9319,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E10" t="n" s="0">
-        <v>28.39877227852286</v>
+        <v>28.398772278522863</v>
       </c>
       <c r="F10" t="n" s="0">
         <v>7.403875948059054</v>
@@ -9348,10 +9348,10 @@
         <v>#NUM!</v>
       </c>
       <c r="E11" t="n" s="0">
-        <v>110.05526962940421</v>
+        <v>110.0552696294042</v>
       </c>
       <c r="F11" t="n" s="0">
-        <v>18.83300006036255</v>
+        <v>18.833000060362554</v>
       </c>
       <c r="G11" t="e" s="0">
         <v>#NUM!</v>
@@ -9406,10 +9406,10 @@
         <v>#NUM!</v>
       </c>
       <c r="E13" t="n" s="0">
-        <v>8.527341601511923</v>
+        <v>8.527341601511925</v>
       </c>
       <c r="F13" t="n" s="0">
-        <v>1.5460740603460157</v>
+        <v>1.546074060346016</v>
       </c>
       <c r="G13" t="e" s="0">
         <v>#NUM!</v>
@@ -9435,7 +9435,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E14" t="n" s="0">
-        <v>0.15167424591158635</v>
+        <v>0.15167424591158632</v>
       </c>
       <c r="F14" t="n" s="0">
         <v>0.3587048494775865</v>
@@ -9464,7 +9464,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E15" t="n" s="0">
-        <v>2.3858717799110485</v>
+        <v>2.385871779911048</v>
       </c>
       <c r="F15" t="n" s="0">
         <v>0.8911856677326341</v>
@@ -9493,7 +9493,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E16" t="n" s="0">
-        <v>7.012965536034739</v>
+        <v>7.0129655360347405</v>
       </c>
       <c r="F16" t="n" s="0">
         <v>2.046097812933876</v>
@@ -9522,7 +9522,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E17" t="n" s="0">
-        <v>3.857404632625341</v>
+        <v>3.8574046326253404</v>
       </c>
       <c r="F17" t="n" s="0">
         <v>1.3243351565015993</v>
@@ -9613,7 +9613,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>0.28691503404526825</v>
+        <v>0.2869150340452683</v>
       </c>
       <c r="D4" t="n" s="0">
         <v>0.4523215640272646</v>
@@ -9671,7 +9671,7 @@
         <v>32</v>
       </c>
       <c r="C6" t="n" s="0">
-        <v>3.5498323827013754</v>
+        <v>3.5498323827013745</v>
       </c>
       <c r="D6" t="n" s="0">
         <v>2.396603053414705</v>
@@ -9700,10 +9700,10 @@
         <v>33</v>
       </c>
       <c r="C7" t="n" s="0">
-        <v>0.055687310972442235</v>
+        <v>0.05568731097244224</v>
       </c>
       <c r="D7" t="n" s="0">
-        <v>0.22931688635837694</v>
+        <v>0.2293168863583769</v>
       </c>
       <c r="E7" t="e" s="0">
         <v>#NUM!</v>
@@ -9758,10 +9758,10 @@
         <v>12</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>5.749297239324742</v>
+        <v>5.749297239324741</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>5.986499736909325</v>
+        <v>5.986499736909326</v>
       </c>
       <c r="E9" t="e" s="0">
         <v>#NUM!</v>
@@ -9790,7 +9790,7 @@
         <v>21.35405419972044</v>
       </c>
       <c r="D10" t="n" s="0">
-        <v>7.640787725890002</v>
+        <v>7.640787725890003</v>
       </c>
       <c r="E10" t="e" s="0">
         <v>#NUM!</v>
@@ -9819,7 +9819,7 @@
         <v>70.89005197430063</v>
       </c>
       <c r="D11" t="n" s="0">
-        <v>13.65796288825613</v>
+        <v>13.657962888256131</v>
       </c>
       <c r="E11" t="e" s="0">
         <v>#NUM!</v>
@@ -9845,10 +9845,10 @@
         <v>35</v>
       </c>
       <c r="C12" t="n" s="0">
-        <v>52.19994931348956</v>
+        <v>52.19994931348957</v>
       </c>
       <c r="D12" t="n" s="0">
-        <v>12.826002079187075</v>
+        <v>12.826002079187074</v>
       </c>
       <c r="E12" t="e" s="0">
         <v>#NUM!</v>
@@ -9877,7 +9877,7 @@
         <v>5.338704233249639</v>
       </c>
       <c r="D13" t="n" s="0">
-        <v>1.5888269726244708</v>
+        <v>1.5888269726244706</v>
       </c>
       <c r="E13" t="e" s="0">
         <v>#NUM!</v>
@@ -9935,7 +9935,7 @@
         <v>1.5784104355055226</v>
       </c>
       <c r="D15" t="n" s="0">
-        <v>1.0276300709187247</v>
+        <v>1.027630070918725</v>
       </c>
       <c r="E15" t="e" s="0">
         <v>#NUM!</v>
@@ -9964,7 +9964,7 @@
         <v>4.905617288089169</v>
       </c>
       <c r="D16" t="n" s="0">
-        <v>0.6804450479256293</v>
+        <v>0.6804450479256294</v>
       </c>
       <c r="E16" t="e" s="0">
         <v>#NUM!</v>
@@ -10122,10 +10122,10 @@
         <v>#NUM!</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>0.03196601960719901</v>
+        <v>0.03196601960719902</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>0.17590961655825182</v>
+        <v>0.17590961655825185</v>
       </c>
       <c r="G5" t="e" s="0">
         <v>#NUM!</v>
@@ -10151,10 +10151,10 @@
         <v>#NUM!</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>3.219482232163374</v>
+        <v>3.2194822321633745</v>
       </c>
       <c r="F6" t="n" s="0">
-        <v>3.3473716942326144</v>
+        <v>3.347371694232615</v>
       </c>
       <c r="G6" t="e" s="0">
         <v>#NUM!</v>
@@ -10209,7 +10209,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E8" t="n" s="0">
-        <v>3.3282071969684743</v>
+        <v>3.3282071969684752</v>
       </c>
       <c r="F8" t="n" s="0">
         <v>3.1535450421298044</v>
@@ -10238,10 +10238,10 @@
         <v>#NUM!</v>
       </c>
       <c r="E9" t="n" s="0">
-        <v>9.978639754261673</v>
+        <v>9.978639754261676</v>
       </c>
       <c r="F9" t="n" s="0">
-        <v>5.919650684911961</v>
+        <v>5.919650684911962</v>
       </c>
       <c r="G9" t="e" s="0">
         <v>#NUM!</v>
@@ -10267,10 +10267,10 @@
         <v>#NUM!</v>
       </c>
       <c r="E10" t="n" s="0">
-        <v>19.07166380241211</v>
+        <v>19.071663802412107</v>
       </c>
       <c r="F10" t="n" s="0">
-        <v>7.839298005628932</v>
+        <v>7.839298005628931</v>
       </c>
       <c r="G10" t="e" s="0">
         <v>#NUM!</v>
@@ -10296,7 +10296,7 @@
         <v>#NUM!</v>
       </c>
       <c r="E11" t="n" s="0">
-        <v>87.9312695862345</v>
+        <v>87.93126958623449</v>
       </c>
       <c r="F11" t="n" s="0">
         <v>20.230947274502082</v>
@@ -10354,10 +10354,10 @@
         <v>#NUM!</v>
       </c>
       <c r="E13" t="n" s="0">
-        <v>6.41788294804295</v>
+        <v>6.417882948042951</v>
       </c>
       <c r="F13" t="n" s="0">
-        <v>2.3582021014234282</v>
+        <v>2.3582021014234287</v>
       </c>
       <c r="G13" t="e" s="0">
         <v>#NUM!</v>
@@ -10415,7 +10415,7 @@
         <v>1.269377658518685</v>
       </c>
       <c r="F15" t="n" s="0">
-        <v>0.9145326074468797</v>
+        <v>0.9145326074468799</v>
       </c>
       <c r="G15" t="e" s="0">
         <v>#NUM!</v>
@@ -10441,10 +10441,10 @@
         <v>#NUM!</v>
       </c>
       <c r="E16" t="n" s="0">
-        <v>6.809611132092428</v>
+        <v>6.809611132092429</v>
       </c>
       <c r="F16" t="n" s="0">
-        <v>1.5267814492567047</v>
+        <v>1.526781449256705</v>
       </c>
       <c r="G16" t="e" s="0">
         <v>#NUM!</v>

</xml_diff>